<commit_message>
remove msw from bid at CF
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,21 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Connecticut\CT-EPS\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF847B7-ADCE-4EF1-B580-1DB5167A7A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="11580"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -133,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,6 +284,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -305,6 +336,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,10 +528,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -586,14 +634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,8 +784,7 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <f>B9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>